<commit_message>
MySqlDatabaseClass.php aangepast en logboek bijgewerkt ook link test db gemaakt
</commit_message>
<xml_diff>
--- a/logboek fotosjaak.xlsx
+++ b/logboek fotosjaak.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
   <si>
     <t>Logboek</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>klasse gemaakt</t>
+  </si>
+  <si>
+    <t>db connectie code gemaakt in de class MySqlDatabaseClass</t>
+  </si>
+  <si>
+    <t>De class MySqlDatabaseClass afgemaakt. Link naar gemaakt in link.php</t>
+  </si>
+  <si>
+    <t>nieuwe link gemaakt test db clas. Op deze pagina een object gemaakt van de MySqlDatabaseClass.</t>
   </si>
   <si>
     <t>weeknr</t>
@@ -115,11 +124,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="D\ MMMM\ YYYY" numFmtId="165"/>
     <numFmt formatCode="HH:MM" numFmtId="166"/>
     <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
+    <numFmt formatCode="DD/MM/YY" numFmtId="168"/>
+    <numFmt formatCode="@" numFmtId="169"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -186,7 +197,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -205,6 +216,22 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0">
+      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -685,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F11" activeCellId="0" pane="topLeft" sqref="F11"/>
+      <selection activeCell="F15" activeCellId="0" pane="topLeft" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -768,13 +795,16 @@
       <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="n">
+        <f aca="false">(D7-C7)</f>
+        <v>0.041666666666666</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="5" t="n">
         <v>0.645833333333333</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="5" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -783,24 +813,76 @@
       <c r="F8" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
-      <c r="F11" s="0" t="s">
+      <c r="G8" s="3" t="inlineStr">
+        <f aca="false">(D8-C8)</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>41607</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0.401388888888889</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <f aca="false">(D9-C9)</f>
+        <v>0.0152777777777778</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="10">
+      <c r="C10" s="2" t="n">
+        <v>0.417361111111111</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <f aca="false">(D10-C10)</f>
+        <v>0.00972222222222219</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="11">
+      <c r="C11" s="3" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
+      <c r="F13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="3" t="n">
-        <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+      <c r="G13" s="3" t="n">
+        <f aca="false">SUM(G7:G10)</f>
+        <v>0.0875</v>
       </c>
     </row>
   </sheetData>
@@ -847,10 +929,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
@@ -867,8 +949,8 @@
         <v>48</v>
       </c>
       <c r="B8" s="3" t="n">
-        <f aca="false">week48!G11</f>
-        <v>0</v>
+        <f aca="false">week48!G13</f>
+        <v>0.0875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
@@ -877,7 +959,7 @@
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0.065277777777778</v>
+        <v>0.152777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>